<commit_message>
ResultsBrowser: updated export & bugs fixed
</commit_message>
<xml_diff>
--- a/examples/DropsTestExample.xlsx
+++ b/examples/DropsTestExample.xlsx
@@ -1,97 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F101A18F-6C07-964D-A539-9A6E09E2C871}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="4620" windowWidth="24560" windowHeight="11680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7380" yWindow="4620" windowWidth="24560" windowHeight="11680" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Testcases" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Testcases" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
-  <si>
-    <t>TFName</t>
-  </si>
-  <si>
-    <t>TFDescription</t>
-  </si>
-  <si>
-    <t>baseURL</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Login 1</t>
-  </si>
-  <si>
-    <t>Login with Username and Password</t>
-  </si>
-  <si>
-    <t>https://app-eu.earthsquad.global/api/rest-auth/login/</t>
-  </si>
-  <si>
-    <t>test151</t>
-  </si>
-  <si>
-    <t>bb140272!</t>
-  </si>
-  <si>
-    <t>Login 2</t>
-  </si>
-  <si>
-    <t>test152</t>
-  </si>
-  <si>
-    <t>TC#</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF008080"/>
       <name val="Menlo"/>
       <charset val="134"/>
+      <b val="1"/>
+      <color rgb="FF008080"/>
+      <sz val="10"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,27 +59,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -389,86 +331,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="42" customWidth="1"/>
+    <col width="33" customWidth="1" min="3" max="3"/>
+    <col width="51.33203125" customWidth="1" min="4" max="4"/>
+    <col width="21.6640625" customWidth="1" min="6" max="6"/>
+    <col width="42" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TC#</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TFName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>TFDescription</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>baseURL</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Login 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Login with Username and Password</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>https://app-eu.earthsquad.global/api/rest-auth/login/</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>test151</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>bb140272!</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Login 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Login with Username and Password</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>https://app-eu.earthsquad.global/api/rest-auth/login/</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>test152</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>bb140272!</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>